<commit_message>
feat: delete users by usernames
</commit_message>
<xml_diff>
--- a/public/input.xlsx
+++ b/public/input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Backend\exam\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C557B3-149D-4B66-90EA-7917066533F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{697373BD-A18D-4AC3-BB7A-F1F56401F2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{95D14BF0-006E-4E26-8CD3-1143D085AE2E}"/>
   </bookViews>
@@ -528,7 +528,7 @@
   <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="N2" sqref="N2:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>

</xml_diff>